<commit_message>
Cập nhật "Cài đặt OpenStack sử dụng PXE và preseed"
</commit_message>
<xml_diff>
--- a/Pike/Use-PXE-preseed/Linuxbridge/images/IP-Planning-Hardware-Requirements.xlsx
+++ b/Pike/Use-PXE-preseed/Linuxbridge/images/IP-Planning-Hardware-Requirements.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VNPT\Install-OpenStack\Pike\Use-PXE-KS\Linuxbridge\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VNPT\Install-OpenStack\Pike\Use-PXE-preseed\Linuxbridge\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -86,9 +86,6 @@
     <t>YÊU CẦU TỐI THIỂU VỀ PHẦN CỨNG LAB</t>
   </si>
   <si>
-    <t>ens4</t>
-  </si>
-  <si>
     <t>10.10.10.72</t>
   </si>
   <si>
@@ -110,9 +107,6 @@
     <t>Compute1</t>
   </si>
   <si>
-    <t>ens5</t>
-  </si>
-  <si>
     <t>192.168.2.61</t>
   </si>
   <si>
@@ -152,13 +146,19 @@
     <t>192.168.2.82</t>
   </si>
   <si>
-    <t>ens3</t>
-  </si>
-  <si>
     <t>172.16.69.101</t>
   </si>
   <si>
     <t>172.16.69.1</t>
+  </si>
+  <si>
+    <t>eth0</t>
+  </si>
+  <si>
+    <t>eth1</t>
+  </si>
+  <si>
+    <t>eth2</t>
   </si>
 </sst>
 </file>
@@ -560,6 +560,120 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="15" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -569,15 +683,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -588,111 +693,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="15" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -980,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C6:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16:J18"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,40 +996,40 @@
   </cols>
   <sheetData>
     <row r="6" spans="3:15" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="C6" s="65" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="66"/>
-      <c r="M6" s="66"/>
-      <c r="N6" s="66"/>
-      <c r="O6" s="67"/>
+      <c r="C6" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="31"/>
     </row>
     <row r="7" spans="3:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="C7" s="68" t="s">
+      <c r="C7" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="70"/>
-      <c r="I7" s="71" t="s">
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="72"/>
-      <c r="K7" s="72"/>
-      <c r="L7" s="72"/>
-      <c r="M7" s="72"/>
-      <c r="N7" s="72"/>
-      <c r="O7" s="73"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="36"/>
+      <c r="O7" s="37"/>
     </row>
     <row r="8" spans="3:15" ht="33" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
@@ -1074,19 +1074,19 @@
     </row>
     <row r="9" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="C9" s="28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>40</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>2</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>9</v>
@@ -1106,7 +1106,7 @@
       <c r="O9" s="21"/>
     </row>
     <row r="10" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C10" s="47" t="s">
+      <c r="C10" s="44" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="6" t="s">
@@ -1116,114 +1116,114 @@
       <c r="F10" s="24"/>
       <c r="G10" s="17"/>
       <c r="H10" s="24"/>
-      <c r="I10" s="52">
+      <c r="I10" s="49">
         <v>6</v>
       </c>
-      <c r="J10" s="43">
+      <c r="J10" s="38">
         <v>2</v>
       </c>
-      <c r="K10" s="32">
+      <c r="K10" s="41">
         <v>50</v>
       </c>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="39"/>
-      <c r="O10" s="39"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="63"/>
+      <c r="N10" s="63"/>
+      <c r="O10" s="63"/>
     </row>
     <row r="11" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C11" s="48"/>
+      <c r="C11" s="45"/>
       <c r="D11" s="11" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F11" s="22" t="s">
         <v>2</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H11" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="53"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="40"/>
-      <c r="M11" s="40"/>
-      <c r="N11" s="40"/>
-      <c r="O11" s="40"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="64"/>
+      <c r="M11" s="64"/>
+      <c r="N11" s="64"/>
+      <c r="O11" s="64"/>
     </row>
     <row r="12" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C12" s="49"/>
+      <c r="C12" s="46"/>
       <c r="D12" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="15" t="s">
         <v>26</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>28</v>
       </c>
       <c r="F12" s="15" t="s">
         <v>2</v>
       </c>
       <c r="G12" s="16"/>
       <c r="H12" s="15"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="41"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="65"/>
+      <c r="M12" s="65"/>
+      <c r="N12" s="65"/>
+      <c r="O12" s="65"/>
     </row>
     <row r="13" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C13" s="56"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="57"/>
-      <c r="L13" s="57"/>
-      <c r="M13" s="57"/>
-      <c r="N13" s="57"/>
-      <c r="O13" s="58"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="54"/>
+      <c r="K13" s="54"/>
+      <c r="L13" s="54"/>
+      <c r="M13" s="54"/>
+      <c r="N13" s="54"/>
+      <c r="O13" s="55"/>
     </row>
     <row r="14" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C14" s="59"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="60"/>
-      <c r="L14" s="60"/>
-      <c r="M14" s="60"/>
-      <c r="N14" s="60"/>
-      <c r="O14" s="61"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="57"/>
+      <c r="K14" s="57"/>
+      <c r="L14" s="57"/>
+      <c r="M14" s="57"/>
+      <c r="N14" s="57"/>
+      <c r="O14" s="58"/>
     </row>
     <row r="15" spans="3:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="62"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
-      <c r="K15" s="63"/>
-      <c r="L15" s="63"/>
-      <c r="M15" s="63"/>
-      <c r="N15" s="63"/>
-      <c r="O15" s="64"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="60"/>
+      <c r="M15" s="60"/>
+      <c r="N15" s="60"/>
+      <c r="O15" s="61"/>
     </row>
     <row r="16" spans="3:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="47" t="s">
-        <v>25</v>
+      <c r="C16" s="44" t="s">
+        <v>24</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>40</v>
@@ -1232,69 +1232,69 @@
       <c r="F16" s="18"/>
       <c r="G16" s="18"/>
       <c r="H16" s="18"/>
-      <c r="I16" s="52">
+      <c r="I16" s="49">
         <v>8</v>
       </c>
-      <c r="J16" s="43">
+      <c r="J16" s="38">
         <v>4</v>
       </c>
-      <c r="K16" s="32">
+      <c r="K16" s="41">
         <v>70</v>
       </c>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29"/>
-      <c r="O16" s="29"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="67"/>
+      <c r="N16" s="67"/>
+      <c r="O16" s="67"/>
     </row>
     <row r="17" spans="3:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="48"/>
+      <c r="C17" s="45"/>
       <c r="D17" s="11" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>2</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H17" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I17" s="53"/>
-      <c r="J17" s="44"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="30"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="68"/>
+      <c r="M17" s="68"/>
+      <c r="N17" s="68"/>
+      <c r="O17" s="68"/>
     </row>
     <row r="18" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C18" s="49"/>
+      <c r="C18" s="46"/>
       <c r="D18" s="14" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F18" s="15" t="s">
         <v>2</v>
       </c>
       <c r="G18" s="16"/>
       <c r="H18" s="15"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="31"/>
-      <c r="O18" s="31"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="69"/>
+      <c r="M18" s="69"/>
+      <c r="N18" s="69"/>
+      <c r="O18" s="69"/>
     </row>
     <row r="19" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C19" s="48" t="s">
-        <v>29</v>
+      <c r="C19" s="45" t="s">
+        <v>27</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>40</v>
@@ -1303,116 +1303,116 @@
       <c r="F19" s="8"/>
       <c r="G19" s="9"/>
       <c r="H19" s="8"/>
-      <c r="I19" s="52">
+      <c r="I19" s="49">
         <v>8</v>
       </c>
-      <c r="J19" s="43">
+      <c r="J19" s="38">
         <v>4</v>
       </c>
-      <c r="K19" s="32">
+      <c r="K19" s="41">
         <v>70</v>
       </c>
-      <c r="L19" s="32"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="32"/>
-      <c r="O19" s="32"/>
+      <c r="L19" s="41"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="41"/>
     </row>
     <row r="20" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C20" s="48"/>
+      <c r="C20" s="45"/>
       <c r="D20" s="11" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>2</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H20" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I20" s="53"/>
-      <c r="J20" s="44"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="33"/>
-      <c r="O20" s="33"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="42"/>
+      <c r="O20" s="42"/>
     </row>
     <row r="21" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C21" s="49"/>
+      <c r="C21" s="46"/>
       <c r="D21" s="14" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F21" s="15" t="s">
         <v>2</v>
       </c>
       <c r="G21" s="16"/>
       <c r="H21" s="15"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="34"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="34"/>
-      <c r="O21" s="34"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="43"/>
+      <c r="O21" s="43"/>
     </row>
     <row r="22" spans="3:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="47" t="s">
-        <v>30</v>
+      <c r="C22" s="44" t="s">
+        <v>28</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="9"/>
       <c r="H22" s="8"/>
-      <c r="I22" s="52"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="32"/>
-      <c r="L22" s="32"/>
-      <c r="M22" s="32"/>
-      <c r="N22" s="32"/>
-      <c r="O22" s="32"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="41"/>
+      <c r="L22" s="41"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
+      <c r="O22" s="41"/>
     </row>
     <row r="23" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C23" s="48"/>
+      <c r="C23" s="45"/>
       <c r="D23" s="11"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
       <c r="G23" s="13"/>
       <c r="H23" s="12"/>
-      <c r="I23" s="53"/>
-      <c r="J23" s="44"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="33"/>
-      <c r="N23" s="33"/>
-      <c r="O23" s="33"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="42"/>
+      <c r="M23" s="42"/>
+      <c r="N23" s="42"/>
+      <c r="O23" s="42"/>
     </row>
     <row r="24" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C24" s="49"/>
+      <c r="C24" s="46"/>
       <c r="D24" s="14"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="16"/>
       <c r="H24" s="15"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="45"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="34"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="34"/>
-      <c r="O24" s="34"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="43"/>
+      <c r="L24" s="43"/>
+      <c r="M24" s="43"/>
+      <c r="N24" s="43"/>
+      <c r="O24" s="43"/>
     </row>
     <row r="25" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C25" s="47" t="s">
-        <v>31</v>
+      <c r="C25" s="44" t="s">
+        <v>29</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>40</v>
@@ -1421,114 +1421,114 @@
       <c r="F25" s="8"/>
       <c r="G25" s="9"/>
       <c r="H25" s="8"/>
-      <c r="I25" s="52">
+      <c r="I25" s="49">
         <v>8</v>
       </c>
-      <c r="J25" s="43">
+      <c r="J25" s="38">
         <v>4</v>
       </c>
-      <c r="K25" s="32">
+      <c r="K25" s="41">
         <v>70</v>
       </c>
-      <c r="L25" s="32"/>
-      <c r="M25" s="32"/>
-      <c r="N25" s="32"/>
-      <c r="O25" s="32"/>
+      <c r="L25" s="41"/>
+      <c r="M25" s="41"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="41"/>
     </row>
     <row r="26" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C26" s="48"/>
+      <c r="C26" s="45"/>
       <c r="D26" s="11" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F26" s="12" t="s">
         <v>2</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H26" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I26" s="53"/>
-      <c r="J26" s="44"/>
-      <c r="K26" s="33"/>
-      <c r="L26" s="33"/>
-      <c r="M26" s="33"/>
-      <c r="N26" s="33"/>
-      <c r="O26" s="33"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="42"/>
+      <c r="L26" s="42"/>
+      <c r="M26" s="42"/>
+      <c r="N26" s="42"/>
+      <c r="O26" s="42"/>
     </row>
     <row r="27" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C27" s="49"/>
+      <c r="C27" s="46"/>
       <c r="D27" s="14" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F27" s="15" t="s">
         <v>2</v>
       </c>
       <c r="G27" s="16"/>
       <c r="H27" s="15"/>
-      <c r="I27" s="54"/>
-      <c r="J27" s="45"/>
-      <c r="K27" s="34"/>
-      <c r="L27" s="34"/>
-      <c r="M27" s="34"/>
-      <c r="N27" s="34"/>
-      <c r="O27" s="34"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="43"/>
+      <c r="M27" s="43"/>
+      <c r="N27" s="43"/>
+      <c r="O27" s="43"/>
     </row>
     <row r="28" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C28" s="56"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="57"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="57"/>
-      <c r="J28" s="57"/>
-      <c r="K28" s="57"/>
-      <c r="L28" s="57"/>
-      <c r="M28" s="57"/>
-      <c r="N28" s="57"/>
-      <c r="O28" s="58"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="54"/>
+      <c r="K28" s="54"/>
+      <c r="L28" s="54"/>
+      <c r="M28" s="54"/>
+      <c r="N28" s="54"/>
+      <c r="O28" s="55"/>
     </row>
     <row r="29" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C29" s="59"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="60"/>
-      <c r="H29" s="60"/>
-      <c r="I29" s="60"/>
-      <c r="J29" s="60"/>
-      <c r="K29" s="60"/>
-      <c r="L29" s="60"/>
-      <c r="M29" s="60"/>
-      <c r="N29" s="60"/>
-      <c r="O29" s="61"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="57"/>
+      <c r="J29" s="57"/>
+      <c r="K29" s="57"/>
+      <c r="L29" s="57"/>
+      <c r="M29" s="57"/>
+      <c r="N29" s="57"/>
+      <c r="O29" s="58"/>
     </row>
     <row r="30" spans="3:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="62"/>
-      <c r="D30" s="63"/>
-      <c r="E30" s="63"/>
-      <c r="F30" s="63"/>
-      <c r="G30" s="63"/>
-      <c r="H30" s="63"/>
-      <c r="I30" s="63"/>
-      <c r="J30" s="63"/>
-      <c r="K30" s="63"/>
-      <c r="L30" s="63"/>
-      <c r="M30" s="63"/>
-      <c r="N30" s="63"/>
-      <c r="O30" s="64"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="60"/>
+      <c r="L30" s="60"/>
+      <c r="M30" s="60"/>
+      <c r="N30" s="60"/>
+      <c r="O30" s="61"/>
     </row>
     <row r="31" spans="3:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="47" t="s">
-        <v>32</v>
+      <c r="C31" s="44" t="s">
+        <v>30</v>
       </c>
       <c r="D31" s="17" t="s">
         <v>40</v>
@@ -1537,73 +1537,73 @@
       <c r="F31" s="18"/>
       <c r="G31" s="18"/>
       <c r="H31" s="18"/>
-      <c r="I31" s="52">
+      <c r="I31" s="49">
         <v>8</v>
       </c>
-      <c r="J31" s="43">
+      <c r="J31" s="38">
         <v>4</v>
       </c>
-      <c r="K31" s="32">
+      <c r="K31" s="41">
         <v>30</v>
       </c>
-      <c r="L31" s="32">
+      <c r="L31" s="41">
         <v>70</v>
       </c>
-      <c r="M31" s="32">
+      <c r="M31" s="41">
         <v>100</v>
       </c>
-      <c r="N31" s="29"/>
-      <c r="O31" s="29"/>
+      <c r="N31" s="67"/>
+      <c r="O31" s="67"/>
     </row>
     <row r="32" spans="3:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="48"/>
+      <c r="C32" s="45"/>
       <c r="D32" s="11" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>2</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H32" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I32" s="53"/>
-      <c r="J32" s="44"/>
-      <c r="K32" s="33"/>
-      <c r="L32" s="33"/>
-      <c r="M32" s="33"/>
-      <c r="N32" s="30"/>
-      <c r="O32" s="30"/>
+      <c r="I32" s="50"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="42"/>
+      <c r="M32" s="42"/>
+      <c r="N32" s="68"/>
+      <c r="O32" s="68"/>
     </row>
     <row r="33" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C33" s="49"/>
+      <c r="C33" s="46"/>
       <c r="D33" s="14" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F33" s="15" t="s">
         <v>2</v>
       </c>
       <c r="G33" s="16"/>
       <c r="H33" s="15"/>
-      <c r="I33" s="54"/>
-      <c r="J33" s="45"/>
-      <c r="K33" s="34"/>
-      <c r="L33" s="34"/>
-      <c r="M33" s="34"/>
-      <c r="N33" s="31"/>
-      <c r="O33" s="31"/>
+      <c r="I33" s="51"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="43"/>
+      <c r="L33" s="43"/>
+      <c r="M33" s="43"/>
+      <c r="N33" s="69"/>
+      <c r="O33" s="69"/>
     </row>
     <row r="34" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C34" s="47" t="s">
-        <v>33</v>
+      <c r="C34" s="44" t="s">
+        <v>31</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>40</v>
@@ -1612,118 +1612,118 @@
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
-      <c r="I34" s="55">
+      <c r="I34" s="52">
         <v>8</v>
       </c>
-      <c r="J34" s="46">
+      <c r="J34" s="62">
         <v>4</v>
       </c>
-      <c r="K34" s="42">
+      <c r="K34" s="66">
         <v>30</v>
       </c>
-      <c r="L34" s="36">
+      <c r="L34" s="71">
         <v>70</v>
       </c>
-      <c r="M34" s="35"/>
-      <c r="N34" s="35"/>
-      <c r="O34" s="35"/>
+      <c r="M34" s="70"/>
+      <c r="N34" s="70"/>
+      <c r="O34" s="70"/>
     </row>
     <row r="35" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C35" s="48"/>
+      <c r="C35" s="45"/>
       <c r="D35" s="11" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F35" s="12" t="s">
         <v>2</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H35" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="I35" s="55"/>
-      <c r="J35" s="46"/>
-      <c r="K35" s="42"/>
-      <c r="L35" s="37"/>
-      <c r="M35" s="35"/>
-      <c r="N35" s="35"/>
-      <c r="O35" s="35"/>
+      <c r="I35" s="52"/>
+      <c r="J35" s="62"/>
+      <c r="K35" s="66"/>
+      <c r="L35" s="72"/>
+      <c r="M35" s="70"/>
+      <c r="N35" s="70"/>
+      <c r="O35" s="70"/>
     </row>
     <row r="36" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C36" s="49"/>
+      <c r="C36" s="46"/>
       <c r="D36" s="14" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F36" s="15" t="s">
         <v>2</v>
       </c>
       <c r="G36" s="16"/>
       <c r="H36" s="20"/>
-      <c r="I36" s="55"/>
-      <c r="J36" s="46"/>
-      <c r="K36" s="42"/>
-      <c r="L36" s="38"/>
-      <c r="M36" s="35"/>
-      <c r="N36" s="35"/>
-      <c r="O36" s="35"/>
+      <c r="I36" s="52"/>
+      <c r="J36" s="62"/>
+      <c r="K36" s="66"/>
+      <c r="L36" s="73"/>
+      <c r="M36" s="70"/>
+      <c r="N36" s="70"/>
+      <c r="O36" s="70"/>
     </row>
     <row r="37" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C37" s="50" t="s">
-        <v>30</v>
+      <c r="C37" s="47" t="s">
+        <v>28</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
       <c r="G37" s="9"/>
       <c r="H37" s="8"/>
-      <c r="I37" s="52"/>
-      <c r="J37" s="43"/>
-      <c r="K37" s="32"/>
-      <c r="L37" s="32"/>
-      <c r="M37" s="32"/>
-      <c r="N37" s="32"/>
-      <c r="O37" s="32"/>
+      <c r="I37" s="49"/>
+      <c r="J37" s="38"/>
+      <c r="K37" s="41"/>
+      <c r="L37" s="41"/>
+      <c r="M37" s="41"/>
+      <c r="N37" s="41"/>
+      <c r="O37" s="41"/>
     </row>
     <row r="38" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C38" s="50"/>
+      <c r="C38" s="47"/>
       <c r="D38" s="11"/>
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
       <c r="G38" s="13"/>
       <c r="H38" s="12"/>
-      <c r="I38" s="53"/>
-      <c r="J38" s="44"/>
-      <c r="K38" s="33"/>
-      <c r="L38" s="33"/>
-      <c r="M38" s="33"/>
-      <c r="N38" s="33"/>
-      <c r="O38" s="33"/>
+      <c r="I38" s="50"/>
+      <c r="J38" s="39"/>
+      <c r="K38" s="42"/>
+      <c r="L38" s="42"/>
+      <c r="M38" s="42"/>
+      <c r="N38" s="42"/>
+      <c r="O38" s="42"/>
     </row>
     <row r="39" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C39" s="51"/>
+      <c r="C39" s="48"/>
       <c r="D39" s="14"/>
       <c r="E39" s="15"/>
       <c r="F39" s="15"/>
       <c r="G39" s="16"/>
       <c r="H39" s="15"/>
-      <c r="I39" s="54"/>
-      <c r="J39" s="45"/>
-      <c r="K39" s="34"/>
-      <c r="L39" s="34"/>
-      <c r="M39" s="34"/>
-      <c r="N39" s="34"/>
-      <c r="O39" s="34"/>
+      <c r="I39" s="51"/>
+      <c r="J39" s="40"/>
+      <c r="K39" s="43"/>
+      <c r="L39" s="43"/>
+      <c r="M39" s="43"/>
+      <c r="N39" s="43"/>
+      <c r="O39" s="43"/>
     </row>
     <row r="40" spans="3:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="47" t="s">
-        <v>34</v>
+      <c r="C40" s="44" t="s">
+        <v>32</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>40</v>
@@ -1732,85 +1732,108 @@
       <c r="F40" s="8"/>
       <c r="G40" s="9"/>
       <c r="H40" s="8"/>
-      <c r="I40" s="52">
+      <c r="I40" s="49">
         <v>8</v>
       </c>
-      <c r="J40" s="43">
+      <c r="J40" s="38">
         <v>4</v>
       </c>
-      <c r="K40" s="32">
+      <c r="K40" s="41">
         <v>30</v>
       </c>
-      <c r="L40" s="32">
+      <c r="L40" s="41">
         <v>70</v>
       </c>
-      <c r="M40" s="32"/>
-      <c r="N40" s="32"/>
-      <c r="O40" s="32"/>
+      <c r="M40" s="41"/>
+      <c r="N40" s="41"/>
+      <c r="O40" s="41"/>
     </row>
     <row r="41" spans="3:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C41" s="48"/>
+      <c r="C41" s="45"/>
       <c r="D41" s="11" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F41" s="12" t="s">
         <v>2</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H41" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I41" s="53"/>
-      <c r="J41" s="44"/>
-      <c r="K41" s="33"/>
-      <c r="L41" s="33"/>
-      <c r="M41" s="33"/>
-      <c r="N41" s="33"/>
-      <c r="O41" s="33"/>
+      <c r="I41" s="50"/>
+      <c r="J41" s="39"/>
+      <c r="K41" s="42"/>
+      <c r="L41" s="42"/>
+      <c r="M41" s="42"/>
+      <c r="N41" s="42"/>
+      <c r="O41" s="42"/>
     </row>
     <row r="42" spans="3:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C42" s="49"/>
+      <c r="C42" s="46"/>
       <c r="D42" s="14" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F42" s="15" t="s">
         <v>2</v>
       </c>
       <c r="G42" s="16"/>
       <c r="H42" s="15"/>
-      <c r="I42" s="54"/>
-      <c r="J42" s="45"/>
-      <c r="K42" s="34"/>
-      <c r="L42" s="34"/>
-      <c r="M42" s="34"/>
-      <c r="N42" s="34"/>
-      <c r="O42" s="34"/>
+      <c r="I42" s="51"/>
+      <c r="J42" s="40"/>
+      <c r="K42" s="43"/>
+      <c r="L42" s="43"/>
+      <c r="M42" s="43"/>
+      <c r="N42" s="43"/>
+      <c r="O42" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="C6:O6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="I7:O7"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="K22:K24"/>
-    <mergeCell ref="K19:K21"/>
-    <mergeCell ref="K16:K18"/>
-    <mergeCell ref="K10:K12"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="J22:J24"/>
-    <mergeCell ref="J19:J21"/>
-    <mergeCell ref="J16:J18"/>
+    <mergeCell ref="O31:O33"/>
+    <mergeCell ref="N31:N33"/>
+    <mergeCell ref="M31:M33"/>
+    <mergeCell ref="L31:L33"/>
+    <mergeCell ref="M40:M42"/>
+    <mergeCell ref="N40:N42"/>
+    <mergeCell ref="O40:O42"/>
+    <mergeCell ref="O37:O39"/>
+    <mergeCell ref="N37:N39"/>
+    <mergeCell ref="M37:M39"/>
+    <mergeCell ref="L40:L42"/>
+    <mergeCell ref="L37:L39"/>
+    <mergeCell ref="O34:O36"/>
+    <mergeCell ref="N34:N36"/>
+    <mergeCell ref="M34:M36"/>
+    <mergeCell ref="L34:L36"/>
+    <mergeCell ref="M25:M27"/>
+    <mergeCell ref="M22:M24"/>
+    <mergeCell ref="M19:M21"/>
+    <mergeCell ref="L25:L27"/>
+    <mergeCell ref="L22:L24"/>
+    <mergeCell ref="L19:L21"/>
+    <mergeCell ref="O25:O27"/>
+    <mergeCell ref="N25:N27"/>
+    <mergeCell ref="O22:O24"/>
+    <mergeCell ref="N22:N24"/>
+    <mergeCell ref="O19:O21"/>
+    <mergeCell ref="N19:N21"/>
+    <mergeCell ref="K40:K42"/>
+    <mergeCell ref="K37:K39"/>
+    <mergeCell ref="K34:K36"/>
+    <mergeCell ref="K31:K33"/>
+    <mergeCell ref="K25:K27"/>
+    <mergeCell ref="J40:J42"/>
+    <mergeCell ref="J37:J39"/>
+    <mergeCell ref="J34:J36"/>
+    <mergeCell ref="J31:J33"/>
+    <mergeCell ref="J25:J27"/>
     <mergeCell ref="C40:C42"/>
     <mergeCell ref="C37:C39"/>
     <mergeCell ref="C34:C36"/>
@@ -1827,52 +1850,29 @@
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="C13:O15"/>
     <mergeCell ref="C28:O30"/>
-    <mergeCell ref="J40:J42"/>
-    <mergeCell ref="J37:J39"/>
-    <mergeCell ref="J34:J36"/>
-    <mergeCell ref="J31:J33"/>
-    <mergeCell ref="J25:J27"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="J22:J24"/>
+    <mergeCell ref="J19:J21"/>
+    <mergeCell ref="J16:J18"/>
+    <mergeCell ref="C6:O6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="I7:O7"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="K22:K24"/>
+    <mergeCell ref="K19:K21"/>
+    <mergeCell ref="K16:K18"/>
+    <mergeCell ref="K10:K12"/>
     <mergeCell ref="O10:O12"/>
     <mergeCell ref="N10:N12"/>
     <mergeCell ref="M10:M12"/>
     <mergeCell ref="L10:L12"/>
-    <mergeCell ref="K40:K42"/>
-    <mergeCell ref="K37:K39"/>
-    <mergeCell ref="K34:K36"/>
-    <mergeCell ref="K31:K33"/>
-    <mergeCell ref="K25:K27"/>
     <mergeCell ref="O16:O18"/>
     <mergeCell ref="N16:N18"/>
     <mergeCell ref="M16:M18"/>
     <mergeCell ref="L16:L18"/>
-    <mergeCell ref="O25:O27"/>
-    <mergeCell ref="N25:N27"/>
-    <mergeCell ref="O22:O24"/>
-    <mergeCell ref="N22:N24"/>
-    <mergeCell ref="O19:O21"/>
-    <mergeCell ref="N19:N21"/>
-    <mergeCell ref="M25:M27"/>
-    <mergeCell ref="M22:M24"/>
-    <mergeCell ref="M19:M21"/>
-    <mergeCell ref="L25:L27"/>
-    <mergeCell ref="L22:L24"/>
-    <mergeCell ref="L19:L21"/>
-    <mergeCell ref="O31:O33"/>
-    <mergeCell ref="N31:N33"/>
-    <mergeCell ref="M31:M33"/>
-    <mergeCell ref="L31:L33"/>
-    <mergeCell ref="M40:M42"/>
-    <mergeCell ref="N40:N42"/>
-    <mergeCell ref="O40:O42"/>
-    <mergeCell ref="O37:O39"/>
-    <mergeCell ref="N37:N39"/>
-    <mergeCell ref="M37:M39"/>
-    <mergeCell ref="L40:L42"/>
-    <mergeCell ref="L37:L39"/>
-    <mergeCell ref="O34:O36"/>
-    <mergeCell ref="N34:N36"/>
-    <mergeCell ref="M34:M36"/>
-    <mergeCell ref="L34:L36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>